<commit_message>
now adding book1 update
</commit_message>
<xml_diff>
--- a/gatting/Book1.xlsx
+++ b/gatting/Book1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ATUL KUMAR\OneDrive\Desktop\calculater\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ATUL KUMAR\OneDrive\Desktop\calculater\gatting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E42F9A5-A44D-4E85-863C-6B4E5D14EAE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6049156-2CFD-4417-8D37-7143792FD75D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4716" yWindow="2052" windowWidth="17280" windowHeight="8964" xr2:uid="{A6574F2C-8269-4FC8-BA92-01B68C7507D3}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve">hi </t>
   </si>
@@ -50,6 +50,18 @@
   </si>
   <si>
     <t>dfsf</t>
+  </si>
+  <si>
+    <t>dfghgfd</t>
+  </si>
+  <si>
+    <t>fghgf</t>
+  </si>
+  <si>
+    <t>try</t>
+  </si>
+  <si>
+    <t>xg</t>
   </si>
 </sst>
 </file>
@@ -401,40 +413,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03398DF8-84DF-4EA4-ACA9-0BFC4951EBB6}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
         <v>5</v>
       </c>
       <c r="E8" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F13" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>